<commit_message>
Fixed number to text issue
</commit_message>
<xml_diff>
--- a/public/Sample.xlsx
+++ b/public/Sample.xlsx
@@ -580,10 +580,157 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -592,68 +739,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -664,9 +754,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -675,93 +762,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1067,8 +1067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36:D36"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1080,269 +1080,269 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="64" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="36"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="66"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="38"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="67"/>
     </row>
     <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="40"/>
-      <c r="C3" s="41" t="s">
+      <c r="B3" s="69"/>
+      <c r="C3" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="42"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="62"/>
+      <c r="I3" s="63"/>
     </row>
     <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="39"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
-      <c r="H4" s="41"/>
-      <c r="I4" s="42"/>
+      <c r="A4" s="68"/>
+      <c r="B4" s="69"/>
+      <c r="C4" s="62"/>
+      <c r="D4" s="62"/>
+      <c r="E4" s="62"/>
+      <c r="F4" s="62"/>
+      <c r="G4" s="62"/>
+      <c r="H4" s="62"/>
+      <c r="I4" s="63"/>
     </row>
     <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="11"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="60"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="9"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="11"/>
+      <c r="A6" s="59"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="60"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="43" t="s">
+      <c r="A7" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="44" t="s">
+      <c r="B7" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="44"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="44"/>
-      <c r="F7" s="45" t="s">
+      <c r="C7" s="49"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="46" t="s">
+      <c r="G7" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="H7" s="46"/>
-      <c r="I7" s="47"/>
+      <c r="H7" s="47"/>
+      <c r="I7" s="48"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="45" t="s">
+      <c r="C8" s="61"/>
+      <c r="D8" s="61"/>
+      <c r="E8" s="61"/>
+      <c r="F8" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G8" s="46">
+      <c r="G8" s="47">
         <v>9821712993</v>
       </c>
-      <c r="H8" s="46"/>
-      <c r="I8" s="47"/>
+      <c r="H8" s="47"/>
+      <c r="I8" s="48"/>
       <c r="J8" s="1"/>
     </row>
     <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="32" t="s">
+      <c r="B9" s="51"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="51"/>
+      <c r="F9" s="51"/>
+      <c r="G9" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="H9" s="32"/>
+      <c r="H9" s="42"/>
       <c r="I9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13" t="s">
+      <c r="B10" s="51"/>
+      <c r="C10" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="32" t="s">
+      <c r="D10" s="51"/>
+      <c r="E10" s="51"/>
+      <c r="F10" s="51"/>
+      <c r="G10" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="H10" s="32"/>
+      <c r="H10" s="42"/>
       <c r="I10" s="6"/>
     </row>
     <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="33" t="s">
+      <c r="A11" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="32"/>
-      <c r="C11" s="32" t="s">
+      <c r="B11" s="42"/>
+      <c r="C11" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="32"/>
+      <c r="D11" s="42"/>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
-      <c r="G11" s="32" t="s">
+      <c r="G11" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="H11" s="32"/>
+      <c r="H11" s="42"/>
       <c r="I11" s="6"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="23" t="s">
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="G12" s="24"/>
-      <c r="H12" s="24"/>
-      <c r="I12" s="25"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="35"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="17"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="27"/>
-      <c r="I13" s="28"/>
+      <c r="A13" s="26"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="38"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="17"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
-      <c r="I14" s="28"/>
+      <c r="A14" s="26"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="38"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="17"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="27"/>
-      <c r="I15" s="28"/>
+      <c r="A15" s="26"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="38"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="20"/>
-      <c r="B16" s="21"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="30"/>
-      <c r="H16" s="30"/>
-      <c r="I16" s="31"/>
+      <c r="A16" s="29"/>
+      <c r="B16" s="30"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="39"/>
+      <c r="G16" s="40"/>
+      <c r="H16" s="40"/>
+      <c r="I16" s="41"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="48" t="s">
+      <c r="A17" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="49" t="s">
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="G17" s="32"/>
-      <c r="H17" s="32"/>
-      <c r="I17" s="50"/>
+      <c r="G17" s="42"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="43"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="43" t="s">
+      <c r="A18" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="51"/>
-      <c r="C18" s="51" t="s">
+      <c r="B18" s="21"/>
+      <c r="C18" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="51"/>
-      <c r="E18" s="51"/>
-      <c r="F18" s="45" t="s">
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="G18" s="51"/>
-      <c r="H18" s="51"/>
-      <c r="I18" s="52"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="22"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="37" t="s">
+      <c r="A19" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13" t="s">
+      <c r="B19" s="51"/>
+      <c r="C19" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="D19" s="13"/>
+      <c r="D19" s="51"/>
       <c r="E19" s="8" t="s">
         <v>37</v>
       </c>
@@ -1355,363 +1355,363 @@
       <c r="H19" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="53" t="s">
+      <c r="I19" s="13" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="54"/>
-      <c r="B20" s="55"/>
-      <c r="C20" s="55"/>
-      <c r="D20" s="56"/>
-      <c r="E20" s="57"/>
-      <c r="F20" s="57"/>
-      <c r="G20" s="57"/>
-      <c r="H20" s="57"/>
-      <c r="I20" s="58"/>
+      <c r="A20" s="17"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="15"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="54"/>
-      <c r="B21" s="55"/>
-      <c r="C21" s="55"/>
-      <c r="D21" s="56"/>
-      <c r="E21" s="57"/>
-      <c r="F21" s="57"/>
-      <c r="G21" s="57"/>
-      <c r="H21" s="57"/>
-      <c r="I21" s="58"/>
+      <c r="A21" s="17"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="15"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="54"/>
-      <c r="B22" s="55"/>
-      <c r="C22" s="55"/>
-      <c r="D22" s="56"/>
-      <c r="E22" s="57"/>
-      <c r="F22" s="57"/>
-      <c r="G22" s="57"/>
-      <c r="H22" s="57"/>
-      <c r="I22" s="58"/>
+      <c r="A22" s="17"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="15"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="54"/>
-      <c r="B23" s="55"/>
-      <c r="C23" s="55"/>
-      <c r="D23" s="56"/>
-      <c r="E23" s="57"/>
-      <c r="F23" s="57"/>
-      <c r="G23" s="57"/>
-      <c r="H23" s="57"/>
-      <c r="I23" s="58"/>
+      <c r="A23" s="17"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="15"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="54"/>
-      <c r="B24" s="55"/>
-      <c r="C24" s="55"/>
-      <c r="D24" s="56"/>
-      <c r="E24" s="57"/>
-      <c r="F24" s="57"/>
-      <c r="G24" s="57"/>
-      <c r="H24" s="57"/>
-      <c r="I24" s="58"/>
+      <c r="A24" s="17"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="15"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="54"/>
-      <c r="B25" s="55"/>
-      <c r="C25" s="55"/>
-      <c r="D25" s="56"/>
-      <c r="E25" s="57"/>
-      <c r="F25" s="57"/>
-      <c r="G25" s="57"/>
-      <c r="H25" s="57"/>
-      <c r="I25" s="58"/>
+      <c r="A25" s="17"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="15"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="54"/>
-      <c r="B26" s="55"/>
-      <c r="C26" s="55"/>
-      <c r="D26" s="56"/>
-      <c r="E26" s="57"/>
-      <c r="F26" s="57"/>
-      <c r="G26" s="57"/>
-      <c r="H26" s="57"/>
-      <c r="I26" s="58"/>
+      <c r="A26" s="17"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="15"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="54"/>
-      <c r="B27" s="55"/>
-      <c r="C27" s="55"/>
-      <c r="D27" s="56"/>
-      <c r="E27" s="57"/>
-      <c r="F27" s="57"/>
-      <c r="G27" s="57"/>
-      <c r="H27" s="57"/>
-      <c r="I27" s="58"/>
+      <c r="A27" s="17"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="15"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="54"/>
-      <c r="B28" s="55"/>
-      <c r="C28" s="55"/>
-      <c r="D28" s="56"/>
-      <c r="E28" s="57"/>
-      <c r="F28" s="57"/>
-      <c r="G28" s="57"/>
-      <c r="H28" s="57"/>
-      <c r="I28" s="58"/>
+      <c r="A28" s="17"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="14"/>
+      <c r="I28" s="15"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="54"/>
-      <c r="B29" s="55"/>
-      <c r="C29" s="55"/>
-      <c r="D29" s="56"/>
-      <c r="E29" s="57"/>
-      <c r="F29" s="57"/>
-      <c r="G29" s="57"/>
-      <c r="H29" s="57"/>
-      <c r="I29" s="58"/>
+      <c r="A29" s="17"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="15"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" s="54"/>
-      <c r="B30" s="55"/>
-      <c r="C30" s="55"/>
-      <c r="D30" s="56"/>
-      <c r="E30" s="57"/>
-      <c r="F30" s="57"/>
-      <c r="G30" s="57"/>
-      <c r="H30" s="57"/>
-      <c r="I30" s="58"/>
+      <c r="A30" s="17"/>
+      <c r="B30" s="18"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="14"/>
+      <c r="I30" s="15"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" s="54"/>
-      <c r="B31" s="55"/>
-      <c r="C31" s="55"/>
-      <c r="D31" s="56"/>
-      <c r="E31" s="57"/>
-      <c r="F31" s="57"/>
-      <c r="G31" s="57"/>
-      <c r="H31" s="57"/>
-      <c r="I31" s="58"/>
+      <c r="A31" s="17"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="15"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" s="54"/>
-      <c r="B32" s="55"/>
-      <c r="C32" s="55"/>
-      <c r="D32" s="56"/>
-      <c r="E32" s="57"/>
-      <c r="F32" s="57"/>
-      <c r="G32" s="57"/>
-      <c r="H32" s="57"/>
-      <c r="I32" s="58"/>
+      <c r="A32" s="17"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="14"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="14"/>
+      <c r="I32" s="15"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" s="54"/>
-      <c r="B33" s="55"/>
-      <c r="C33" s="55"/>
-      <c r="D33" s="56"/>
-      <c r="E33" s="57"/>
-      <c r="F33" s="57"/>
-      <c r="G33" s="57"/>
-      <c r="H33" s="57"/>
-      <c r="I33" s="58"/>
+      <c r="A33" s="17"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="14"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="14"/>
+      <c r="I33" s="15"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" s="54"/>
-      <c r="B34" s="55"/>
-      <c r="C34" s="55"/>
-      <c r="D34" s="56"/>
-      <c r="E34" s="57"/>
-      <c r="F34" s="57"/>
-      <c r="G34" s="57"/>
-      <c r="H34" s="57"/>
-      <c r="I34" s="58"/>
+      <c r="A34" s="17"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="14"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="14"/>
+      <c r="I34" s="15"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A35" s="54"/>
-      <c r="B35" s="55"/>
-      <c r="C35" s="55"/>
-      <c r="D35" s="56"/>
-      <c r="E35" s="57"/>
-      <c r="F35" s="57"/>
-      <c r="G35" s="57"/>
-      <c r="H35" s="57"/>
-      <c r="I35" s="58"/>
+      <c r="A35" s="17"/>
+      <c r="B35" s="18"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="14"/>
+      <c r="I35" s="15"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A36" s="54"/>
-      <c r="B36" s="55"/>
-      <c r="C36" s="55"/>
-      <c r="D36" s="56"/>
-      <c r="E36" s="57"/>
-      <c r="F36" s="57"/>
-      <c r="G36" s="57"/>
-      <c r="H36" s="57"/>
-      <c r="I36" s="58"/>
+      <c r="A36" s="17"/>
+      <c r="B36" s="18"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
+      <c r="G36" s="14"/>
+      <c r="H36" s="14"/>
+      <c r="I36" s="15"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" s="54"/>
-      <c r="B37" s="55"/>
-      <c r="C37" s="55"/>
-      <c r="D37" s="56"/>
-      <c r="E37" s="57"/>
-      <c r="F37" s="57"/>
-      <c r="G37" s="57"/>
-      <c r="H37" s="57"/>
-      <c r="I37" s="58"/>
+      <c r="A37" s="17"/>
+      <c r="B37" s="18"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="14"/>
+      <c r="H37" s="14"/>
+      <c r="I37" s="15"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A38" s="54"/>
-      <c r="B38" s="55"/>
-      <c r="C38" s="55"/>
-      <c r="D38" s="56"/>
-      <c r="E38" s="57"/>
-      <c r="F38" s="57"/>
-      <c r="G38" s="57"/>
-      <c r="H38" s="57"/>
-      <c r="I38" s="58"/>
+      <c r="A38" s="17"/>
+      <c r="B38" s="18"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="14"/>
+      <c r="H38" s="14"/>
+      <c r="I38" s="15"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A39" s="59" t="s">
+      <c r="A39" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="B39" s="60"/>
-      <c r="C39" s="60"/>
-      <c r="D39" s="60"/>
-      <c r="E39" s="60"/>
-      <c r="F39" s="60"/>
-      <c r="G39" s="61" t="s">
+      <c r="B39" s="46"/>
+      <c r="C39" s="46"/>
+      <c r="D39" s="46"/>
+      <c r="E39" s="46"/>
+      <c r="F39" s="46"/>
+      <c r="G39" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="H39" s="61"/>
-      <c r="I39" s="58"/>
+      <c r="H39" s="20"/>
+      <c r="I39" s="15"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A40" s="59"/>
-      <c r="B40" s="60"/>
-      <c r="C40" s="60"/>
-      <c r="D40" s="60"/>
-      <c r="E40" s="60"/>
-      <c r="F40" s="60"/>
-      <c r="G40" s="61" t="s">
+      <c r="A40" s="45"/>
+      <c r="B40" s="46"/>
+      <c r="C40" s="46"/>
+      <c r="D40" s="46"/>
+      <c r="E40" s="46"/>
+      <c r="F40" s="46"/>
+      <c r="G40" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="H40" s="61"/>
-      <c r="I40" s="58"/>
+      <c r="H40" s="20"/>
+      <c r="I40" s="15"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A41" s="59"/>
-      <c r="B41" s="60"/>
-      <c r="C41" s="60"/>
-      <c r="D41" s="60"/>
-      <c r="E41" s="60"/>
-      <c r="F41" s="60"/>
-      <c r="G41" s="61" t="s">
+      <c r="A41" s="45"/>
+      <c r="B41" s="46"/>
+      <c r="C41" s="46"/>
+      <c r="D41" s="46"/>
+      <c r="E41" s="46"/>
+      <c r="F41" s="46"/>
+      <c r="G41" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="H41" s="61"/>
-      <c r="I41" s="58"/>
+      <c r="H41" s="20"/>
+      <c r="I41" s="15"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A42" s="59" t="s">
+      <c r="A42" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="B42" s="60"/>
-      <c r="C42" s="60"/>
-      <c r="D42" s="60"/>
-      <c r="E42" s="60"/>
-      <c r="F42" s="60"/>
-      <c r="G42" s="61" t="s">
+      <c r="B42" s="46"/>
+      <c r="C42" s="46"/>
+      <c r="D42" s="46"/>
+      <c r="E42" s="46"/>
+      <c r="F42" s="46"/>
+      <c r="G42" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="H42" s="61"/>
-      <c r="I42" s="58"/>
+      <c r="H42" s="20"/>
+      <c r="I42" s="15"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A43" s="59"/>
-      <c r="B43" s="60"/>
-      <c r="C43" s="60"/>
-      <c r="D43" s="60"/>
-      <c r="E43" s="60"/>
-      <c r="F43" s="60"/>
-      <c r="G43" s="61" t="s">
+      <c r="A43" s="45"/>
+      <c r="B43" s="46"/>
+      <c r="C43" s="46"/>
+      <c r="D43" s="46"/>
+      <c r="E43" s="46"/>
+      <c r="F43" s="46"/>
+      <c r="G43" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="H43" s="61"/>
-      <c r="I43" s="58"/>
+      <c r="H43" s="20"/>
+      <c r="I43" s="15"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A44" s="59"/>
-      <c r="B44" s="60"/>
-      <c r="C44" s="60"/>
-      <c r="D44" s="60"/>
-      <c r="E44" s="60"/>
-      <c r="F44" s="60"/>
-      <c r="G44" s="61" t="s">
+      <c r="A44" s="45"/>
+      <c r="B44" s="46"/>
+      <c r="C44" s="46"/>
+      <c r="D44" s="46"/>
+      <c r="E44" s="46"/>
+      <c r="F44" s="46"/>
+      <c r="G44" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="H44" s="61"/>
-      <c r="I44" s="58"/>
+      <c r="H44" s="20"/>
+      <c r="I44" s="15"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A45" s="43" t="s">
+      <c r="A45" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="61"/>
-      <c r="C45" s="61"/>
-      <c r="D45" s="61"/>
-      <c r="E45" s="61"/>
-      <c r="F45" s="61"/>
-      <c r="G45" s="60" t="s">
+      <c r="B45" s="20"/>
+      <c r="C45" s="20"/>
+      <c r="D45" s="20"/>
+      <c r="E45" s="20"/>
+      <c r="F45" s="20"/>
+      <c r="G45" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="H45" s="60"/>
-      <c r="I45" s="62"/>
+      <c r="H45" s="46"/>
+      <c r="I45" s="52"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A46" s="63" t="s">
+      <c r="A46" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="B46" s="61"/>
-      <c r="C46" s="61"/>
-      <c r="D46" s="61"/>
-      <c r="E46" s="61"/>
-      <c r="F46" s="61"/>
-      <c r="G46" s="60"/>
-      <c r="H46" s="60"/>
-      <c r="I46" s="62"/>
+      <c r="B46" s="20"/>
+      <c r="C46" s="20"/>
+      <c r="D46" s="20"/>
+      <c r="E46" s="20"/>
+      <c r="F46" s="20"/>
+      <c r="G46" s="46"/>
+      <c r="H46" s="46"/>
+      <c r="I46" s="52"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A47" s="59" t="s">
+      <c r="A47" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="B47" s="64"/>
-      <c r="C47" s="64"/>
-      <c r="D47" s="64"/>
-      <c r="E47" s="64"/>
-      <c r="F47" s="64"/>
-      <c r="G47" s="60"/>
-      <c r="H47" s="60"/>
-      <c r="I47" s="62"/>
+      <c r="B47" s="55"/>
+      <c r="C47" s="55"/>
+      <c r="D47" s="55"/>
+      <c r="E47" s="55"/>
+      <c r="F47" s="55"/>
+      <c r="G47" s="46"/>
+      <c r="H47" s="46"/>
+      <c r="I47" s="52"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A48" s="65"/>
-      <c r="B48" s="64"/>
-      <c r="C48" s="64"/>
-      <c r="D48" s="64"/>
-      <c r="E48" s="64"/>
-      <c r="F48" s="64"/>
-      <c r="G48" s="60"/>
-      <c r="H48" s="60"/>
-      <c r="I48" s="62"/>
+      <c r="A48" s="56"/>
+      <c r="B48" s="55"/>
+      <c r="C48" s="55"/>
+      <c r="D48" s="55"/>
+      <c r="E48" s="55"/>
+      <c r="F48" s="55"/>
+      <c r="G48" s="46"/>
+      <c r="H48" s="46"/>
+      <c r="I48" s="52"/>
     </row>
     <row r="49" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="66"/>
-      <c r="B49" s="67"/>
-      <c r="C49" s="67"/>
-      <c r="D49" s="67"/>
-      <c r="E49" s="67"/>
-      <c r="F49" s="67"/>
-      <c r="G49" s="68"/>
-      <c r="H49" s="68"/>
-      <c r="I49" s="69"/>
+      <c r="A49" s="57"/>
+      <c r="B49" s="58"/>
+      <c r="C49" s="58"/>
+      <c r="D49" s="58"/>
+      <c r="E49" s="58"/>
+      <c r="F49" s="58"/>
+      <c r="G49" s="53"/>
+      <c r="H49" s="53"/>
+      <c r="I49" s="54"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="G50" s="2"/>
@@ -1720,12 +1720,37 @@
     </row>
   </sheetData>
   <mergeCells count="53">
-    <mergeCell ref="A38:D38"/>
-    <mergeCell ref="A32:D32"/>
-    <mergeCell ref="A33:D33"/>
-    <mergeCell ref="A34:D34"/>
-    <mergeCell ref="A35:D35"/>
-    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="A5:I6"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="C3:I4"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A3:B4"/>
+    <mergeCell ref="A42:F44"/>
+    <mergeCell ref="A39:F41"/>
+    <mergeCell ref="B46:F46"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="G41:H41"/>
+    <mergeCell ref="G42:H42"/>
+    <mergeCell ref="G43:H43"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="G45:I49"/>
+    <mergeCell ref="A47:F49"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="A12:E16"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="F12:I16"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="G11:H11"/>
     <mergeCell ref="B45:F45"/>
     <mergeCell ref="B18:E18"/>
     <mergeCell ref="G18:I18"/>
@@ -1742,37 +1767,12 @@
     <mergeCell ref="A30:D30"/>
     <mergeCell ref="A31:D31"/>
     <mergeCell ref="A37:D37"/>
-    <mergeCell ref="A12:E16"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="F12:I16"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="A42:F44"/>
-    <mergeCell ref="A39:F41"/>
-    <mergeCell ref="B46:F46"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="G41:H41"/>
-    <mergeCell ref="G42:H42"/>
-    <mergeCell ref="G43:H43"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="G45:I49"/>
-    <mergeCell ref="A47:F49"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="A5:I6"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="C3:I4"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A3:B4"/>
+    <mergeCell ref="A38:D38"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="A33:D33"/>
+    <mergeCell ref="A34:D34"/>
+    <mergeCell ref="A35:D35"/>
+    <mergeCell ref="A36:D36"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1"/>

</xml_diff>